<commit_message>
Added Account creation page
</commit_message>
<xml_diff>
--- a/resource/TestData/LogIn.xlsx
+++ b/resource/TestData/LogIn.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\eclipse-workspace\myStore\resource\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="AccountCreation" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
   <si>
     <t>UserName</t>
   </si>
@@ -36,13 +37,136 @@
   </si>
   <si>
     <t>milan@123</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Telephone</t>
+  </si>
+  <si>
+    <t>Fax</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Address1</t>
+  </si>
+  <si>
+    <t>Address2</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>LogInName</t>
+  </si>
+  <si>
+    <t>Milan</t>
+  </si>
+  <si>
+    <t>Sutar</t>
+  </si>
+  <si>
+    <t>test1@email.com</t>
+  </si>
+  <si>
+    <t>tcs</t>
+  </si>
+  <si>
+    <t>bbsr</t>
+  </si>
+  <si>
+    <t>ctc</t>
+  </si>
+  <si>
+    <t>Orissa</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Milan79782</t>
+  </si>
+  <si>
+    <t>Milan@123</t>
+  </si>
+  <si>
+    <t>Tarun</t>
+  </si>
+  <si>
+    <t>Priyadarshi</t>
+  </si>
+  <si>
+    <t>test2@fmail.com</t>
+  </si>
+  <si>
+    <t>infosys</t>
+  </si>
+  <si>
+    <t>bhub</t>
+  </si>
+  <si>
+    <t>Goa</t>
+  </si>
+  <si>
+    <t>Tarun79782</t>
+  </si>
+  <si>
+    <t>Tarun@123</t>
+  </si>
+  <si>
+    <t>Gudu</t>
+  </si>
+  <si>
+    <t>Maharana</t>
+  </si>
+  <si>
+    <t>test3@hmail.com</t>
+  </si>
+  <si>
+    <t>HCL</t>
+  </si>
+  <si>
+    <t>Rusikesh</t>
+  </si>
+  <si>
+    <t>sikher</t>
+  </si>
+  <si>
+    <t>Jalandar</t>
+  </si>
+  <si>
+    <t>Punjab</t>
+  </si>
+  <si>
+    <t>Gudu79782</t>
+  </si>
+  <si>
+    <t>Gudu@123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,8 +182,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -69,6 +201,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -86,10 +224,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -373,7 +514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -405,4 +546,207 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <v>5555566666</v>
+      </c>
+      <c r="E2">
+        <v>6666655555</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2">
+        <v>751021</v>
+      </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3">
+        <v>7777799999</v>
+      </c>
+      <c r="E3">
+        <v>9999977777</v>
+      </c>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3">
+        <v>654345</v>
+      </c>
+      <c r="L3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4">
+        <v>1111188888</v>
+      </c>
+      <c r="E4">
+        <v>8888811111</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4">
+        <v>654234</v>
+      </c>
+      <c r="L4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>